<commit_message>
add internationalisation feature with an excel file to translate. Not yet finished. But tested ok. Debug of remove camp from radar plot for notes.
</commit_message>
<xml_diff>
--- a/webapp/config_notes_isolement.xlsx
+++ b/webapp/config_notes_isolement.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\camps\webapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B0FCC3-779C-42BA-A7AC-8A3A881C7F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBD2C59-4A00-44CA-A59E-82E8773C2A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31DD1F19-F79B-4F44-981A-EF4A7B1E6F45}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{31DD1F19-F79B-4F44-981A-EF4A7B1E6F45}"/>
   </bookViews>
   <sheets>
     <sheet name="2024-11-25_indices_isolement" sheetId="1" r:id="rId1"/>
+    <sheet name="traductions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="124">
   <si>
     <t>Test indicateur d'isolement</t>
   </si>
@@ -118,13 +119,330 @@
   </si>
   <si>
     <t>atm_distance</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>actions</t>
+  </si>
+  <si>
+    <t>add_camp</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>clear_radar</t>
+  </si>
+  <si>
+    <t>camp_type</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>suburb</t>
+  </si>
+  <si>
+    <t>rural</t>
+  </si>
+  <si>
+    <t>not_classified</t>
+  </si>
+  <si>
+    <t>not_verified</t>
+  </si>
+  <si>
+    <t>active_camps</t>
+  </si>
+  <si>
+    <t>inactive_camps</t>
+  </si>
+  <si>
+    <t>dist_profile</t>
+  </si>
+  <si>
+    <t>note_profile</t>
+  </si>
+  <si>
+    <t>map_title</t>
+  </si>
+  <si>
+    <t>add_title</t>
+  </si>
+  <si>
+    <t>add_subtitle</t>
+  </si>
+  <si>
+    <t>add_warning</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>verification</t>
+  </si>
+  <si>
+    <t>captcha_placeholder</t>
+  </si>
+  <si>
+    <t>error_captcha</t>
+  </si>
+  <si>
+    <t>error_semicolon</t>
+  </si>
+  <si>
+    <t>success_add</t>
+  </si>
+  <si>
+    <t>about_text</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>keys</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Geographical Analysis of Migrant Camps in Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Interactive mapping and analysis of distances to essential infrastructures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Add a new camp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> About</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clear radar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Camp type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> City</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Suburb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rural</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Not classified</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Not verified</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Active camps</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inactive camps</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Distance profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Score profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Map of migrant camps in and around Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ➕ Add a new camp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fill in the information below</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Do not enter semicolons (;) in the fields else the entry will be refused</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✓ Save</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ← Cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enter the answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verification error  : the captcha answer is incorrect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Error :  field '{key}' contains a semicolon which is not allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The camp has been successfully added and saved.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Analyse Géographique des Camps de Migrants en Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cartographie interactive et analyse des distances aux infrastructures essentielles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ajouter un nouveau camp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> À propos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vider le radar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Type de camp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ville</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Banlieue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Non classifié</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Non vérifié</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Camps actifs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Camps désaffectés</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Profil des distances</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Profil des notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carte des camps pour migrants en Europe et autour</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ➕ Ajouter un nouveau camp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remplissez les informations ci-dessous</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ne saisissez pas de point-virgules (;) dans les champs sinon la saisie sera refusée</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✓ Enregistrer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ← Annuler</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vérification</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Entrez la réponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Erreur de vérification : la réponse au captcha est incorrecte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Erreur :  le champ '{key}' contient un point-virgule ce qui n'est pas autorisé.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Le camp a bien été ajouté et enregistré.</t>
+  </si>
+  <si>
+    <t>radar_title</t>
+  </si>
+  <si>
+    <t>Remoteness from socio-environmental amenities</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>É</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>loignement des aménités socio-environnementales</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cette application propose une visualisation interactive des camps en Europe base de données complétée et qualifiée de mars 2025 en collaboration avec Louis Fernier doctorant à Migrinter.
+L'application a été développée dans le cadre du Master 2 SPE à La Rochelle UE Data to Information en décembre 2025 sous la responsabilité de Christine Plumejeaud-Perreau enseignante de l'UE par des étudiants du Master 2 SPE :
+&lt;ul&gt;&lt;li&gt;Damien Glo&lt;/li&gt;&lt;li&gt;Killian Lheote&lt;/li&gt;&lt;li&gt;Joseph Fournier.&lt;/li&gt;&lt;/ul&gt;
+&lt;br&gt;
+C'est un prototype visant à démontrer les capacités d'exploration et visualisation des profils des camps avec Python (3.10). Il nécessite des améliorations pour une utilisation en production (en particulier pour le formulaire de saisie de nouveaux camps qui ne fonctionne pas).&lt;br&gt;
+Développé avec Flask Folium et Plotly le code source est disponible sur le github de l'enseignante sous licence Affero GPL v3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This application offers an interactive visualization of camps in Europe database completed and qualified in March 2025 in collaboration with Louis Fernier PhD student at Migrinter. The application was developed as part of the Master 2 SPE at La Rochelle UE Data to Information in December 2025 under the responsibility of Christine Plumejeaud-Perreau course instructor by students of the Master 2 SPE:
+&lt;ul&gt;&lt;li&gt;Damien Glo&lt;/li&gt;&lt;li&gt;Killian Lheote&lt;/li&gt;&lt;li&gt;Joseph Fournier.&lt;/li&gt;&lt;/ul&gt;
+&lt;br&gt;
+This is a prototype to demonstrate the exploration and visualization capabilities of camp profiles with Python (3.10). It requires improvements for production use (especially for the new camp entry form which does not work yet).&lt;br&gt;
+Developed with Flask Folium and Plotly the source code is available on the teacher's github under the Affero GPL v3 license.</t>
+  </si>
+  <si>
+    <t>camp_classification</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classified as </t>
+  </si>
+  <si>
+    <t>Masquer du radar</t>
+  </si>
+  <si>
+    <t>Remove from radar</t>
+  </si>
+  <si>
+    <t>remove_from_radar</t>
+  </si>
+  <si>
+    <t>add_to_radar</t>
+  </si>
+  <si>
+    <t>Voir dans le radar</t>
+  </si>
+  <si>
+    <t>Add to radar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +483,34 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA31515"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +520,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,7 +824,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
@@ -552,6 +902,31 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -870,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FBD2F8-1BE0-474F-8D4E-191BBCFAC4F3}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,4 +2386,400 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233F7D4F-ED1F-40B9-822C-B32E141787E6}">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="43"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>